<commit_message>
Parsing 1 job to xlsx file
</commit_message>
<xml_diff>
--- a/Job_template.xlsx
+++ b/Job_template.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId3"/>
     <sheet name="Sections" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="479">
   <si>
     <t>EDTFILE:outbound:</t>
   </si>
@@ -1498,11 +1498,20 @@
   <si>
     <t>OFCOM false positive rate</t>
   </si>
+  <si>
+    <t>Percentage complete of job to trigger callsel of link job</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>Automatically start Update mode on customer hang up</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1858,10 +1867,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1871,12 +1886,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2158,7 +2167,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2166,10 +2175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,156 +2189,149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="str">
-        <f>LEFT(B1,FIND(":",B1)-1)</f>
-        <v>ANI</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1">
-        <f>FIND("I",B1)</f>
-        <v>3</v>
+      <c r="A1" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="str">
-        <f t="shared" ref="A2:A65" si="0">LEFT(B2,FIND(":",B2)-1)</f>
-        <v>ANI_FIELD</v>
+        <f t="shared" ref="A2:A5" si="0">LEFT(B2,FIND(":",B2)-1)</f>
+        <v>JLABEL</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>9</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>AUTOCALLSEL_TRIGGER</v>
+        <v>STARTTIME</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>138</v>
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>JLABEL</v>
+        <v>STOPTIME</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>93</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="str">
         <f t="shared" si="0"/>
-        <v>LOGONUNIT</v>
+        <v>PORTS</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>474</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>PORTS</v>
+        <f>LEFT(B6,FIND(":",B6)-1)</f>
+        <v>ANI</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>92</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <f>FIND("I",B6)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>STARTTIME</v>
+        <f t="shared" ref="A7:A66" si="1">LEFT(B7,FIND(":",B7)-1)</f>
+        <v>ANI_FIELD</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>88</v>
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>STOPTIME</v>
+        <f t="shared" si="1"/>
+        <v>AUTOCALLSEL_TRIGGER</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>89</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>TRANSID</v>
+        <f t="shared" si="1"/>
+        <v>LOGONUNIT</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>95</v>
+        <v>16</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>TRANSID</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>TRANSTAT</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>CPMETHOD</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>ECPA</v>
+        <f t="shared" si="1"/>
+        <v>CPMETHOD</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>100</v>
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>HITRATE</v>
       </c>
       <c r="B13" s="20" t="s">
@@ -2341,7 +2343,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>IDMODE</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -2353,7 +2355,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>MINHITRATE</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -2364,84 +2366,84 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>DNC_GROUP</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>25</v>
+      <c r="A16" s="20" t="str">
+        <f t="shared" ref="A16:A18" si="2">LEFT(B16,FIND(":",B16)-1)</f>
+        <v>ECPA</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>LINKJOB</v>
+        <f t="shared" si="2"/>
+        <v>LIST</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>LIST</v>
+        <f t="shared" si="2"/>
+        <v>SELECT</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>OKEYS</v>
+        <f t="shared" si="1"/>
+        <v>DNC_GROUP</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>SCREEN</v>
+        <f t="shared" si="1"/>
+        <v>OKEYS</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>SELECT</v>
+        <f t="shared" si="1"/>
+        <v>SCREEN</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
+        <v>103</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>TRANSFER_TO_JOB</v>
       </c>
       <c r="B22" s="25" t="s">
@@ -2456,31 +2458,27 @@
       <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>IVR_AGENTS</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>74</v>
+      <c r="A23" s="25" t="str">
+        <f t="shared" ref="A23" si="3">LEFT(B23,FIND(":",B23)-1)</f>
+        <v>OKEYS</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
+        <v>104</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>IVR_ID</v>
+        <f t="shared" si="1"/>
+        <v>IVR_AGENTS</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
@@ -2489,14 +2487,14 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>IVR_INITSCRIPT</v>
+        <f t="shared" si="1"/>
+        <v>IVR_ID</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
@@ -2505,14 +2503,14 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="str">
-        <f t="shared" si="0"/>
-        <v>IVR_SCRIPT</v>
+        <f t="shared" si="1"/>
+        <v>IVR_INITSCRIPT</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
@@ -2520,15 +2518,15 @@
       <c r="H26" s="22"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>FCC</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>5</v>
+      <c r="A27" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>IVR_SCRIPT</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>77</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
@@ -2537,14 +2535,14 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>OFCOM</v>
+        <f t="shared" ref="A28" si="4">LEFT(B28,FIND(":",B28)-1)</f>
+        <v>TRANJOB</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
@@ -2553,14 +2551,14 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>TRANJOB</v>
+        <f t="shared" ref="A29" si="5">LEFT(B29,FIND(":",B29)-1)</f>
+        <v>VIRTUAL</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
@@ -2569,40 +2567,40 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>OFCOM_METHOD</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="1"/>
+        <f t="shared" si="1"/>
+        <v>OFCOM</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>VIRTUAL</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
+        <f t="shared" si="1"/>
+        <v>OFCOM_METHOD</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="str">
-        <f t="shared" si="0"/>
-        <v>DATAPROCESS</v>
-      </c>
-      <c r="B32" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>117</v>
+      <c r="A32" s="36" t="str">
+        <f t="shared" ref="A32:A33" si="6">LEFT(B32,FIND(":",B32)-1)</f>
+        <v>FCC</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
@@ -2611,7 +2609,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>RUNCALL</v>
       </c>
       <c r="B33" s="35" t="s">
@@ -2626,15 +2624,15 @@
       <c r="H33" s="22"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>PVCANCEL</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>125</v>
+      <c r="A34" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>DATAPROCESS</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
@@ -2643,7 +2641,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A35" si="7">LEFT(B35,FIND(":",B35)-1)</f>
         <v>PVDIAL</v>
       </c>
       <c r="B35" s="38" t="s">
@@ -2659,14 +2657,14 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>PVEMPTYREC</v>
+        <f t="shared" si="1"/>
+        <v>PVCANCEL</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
@@ -2675,14 +2673,14 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>PVIGNOREDEL</v>
+        <f t="shared" si="1"/>
+        <v>PVEMPTYREC</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>128</v>
+        <v>60</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
@@ -2691,615 +2689,631 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>PVKEYFLD</v>
+        <f t="shared" si="1"/>
+        <v>PVIGNOREDEL</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>130</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>PVLENGTH</v>
+        <f t="shared" si="1"/>
+        <v>PVKEYFLD</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>PVLENGTH</v>
+      </c>
+      <c r="B40" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="38" t="str">
+        <f t="shared" si="1"/>
         <v>PVSEARCHTYPE</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B41" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v>JOBEND</v>
-      </c>
-      <c r="B41" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v>LOWALTQPRIO</v>
+        <f t="shared" si="1"/>
+        <v>JOBEND</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>460</v>
+        <v>42</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v>MAKE_CALL_VDN</v>
+        <f t="shared" si="1"/>
+        <v>LOWALTQPRIO</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>449</v>
+        <v>43</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>MAKE_CALL_VDN</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="40" t="str">
+        <f t="shared" si="1"/>
         <v>ORDERZONES</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B45" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>452</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="str">
-        <f t="shared" si="0"/>
-        <v>AUTORELEASE</v>
-      </c>
-      <c r="B45" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>AUTORELEASE</v>
+      </c>
+      <c r="B46" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="44" t="str">
+        <f t="shared" si="1"/>
         <v>POSTUPDATE</v>
       </c>
-      <c r="B46" s="44" t="s">
+      <c r="B47" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>QUOTA_EXTFILE</v>
-      </c>
-      <c r="B47" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>QUOTA_SAVE</v>
+        <f t="shared" si="1"/>
+        <v>QUOTA_EXTFILE</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="42" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>QUOTA_SAVE</v>
+      </c>
+      <c r="B49" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="42" t="str">
+        <f t="shared" si="1"/>
         <v>QUOTAVAL</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B50" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>453</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>INF_ESC_RECALL</v>
-      </c>
-      <c r="B50" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>INF_RECALL_GETOP_JOB</v>
+        <f t="shared" si="1"/>
+        <v>INF_ESC_RECALL</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>RECALL_CPA</v>
+        <f t="shared" si="1"/>
+        <v>INF_RECALL_GETOP_JOB</v>
       </c>
       <c r="B52" s="27" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>RECALL_INTERVAL</v>
+        <f t="shared" si="1"/>
+        <v>RECALL_CPA</v>
       </c>
       <c r="B53" s="27" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>RECALL_NOTIFY</v>
+        <f t="shared" si="1"/>
+        <v>RECALL_INTERVAL</v>
       </c>
       <c r="B54" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>RECALL_NOTIFY</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="27" t="str">
+        <f t="shared" si="1"/>
         <v>RECALL_NUMOFTRY</v>
       </c>
-      <c r="B55" s="27" t="s">
+      <c r="B56" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v>OFCOMTIMER</v>
-      </c>
-      <c r="B56" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
-      <c r="H56" s="22"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v>OFCOMFR</v>
+        <f t="shared" si="1"/>
+        <v>OFCOMTIMER</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>87</v>
+        <v>8</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>475</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="22"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="34" t="str">
-        <f t="shared" si="0"/>
-        <v>CONNTOLE</v>
+        <f t="shared" si="1"/>
+        <v>OFCOMFR</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>99</v>
+        <v>87</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>CONNTOLE</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="34" t="str">
+        <f t="shared" si="1"/>
         <v>SERVICELEVEL</v>
       </c>
-      <c r="B59" s="34" t="s">
+      <c r="B60" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="50" t="str">
-        <f t="shared" si="0"/>
-        <v>WAITLIMIT</v>
-      </c>
-      <c r="B60" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="50" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>WAITLIMIT</v>
+      </c>
+      <c r="B61" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="50" t="str">
+        <f t="shared" si="1"/>
         <v>XFERHOLDMSGNO</v>
       </c>
-      <c r="B61" s="50" t="s">
+      <c r="B62" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="47" t="s">
+      <c r="C62" s="47" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="37" t="str">
-        <f t="shared" si="0"/>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="37" t="str">
+        <f t="shared" si="1"/>
         <v>AUTOEND</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="str">
-        <f t="shared" si="0"/>
-        <v>AUTOREL_AGTRDY_METHOD</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f t="shared" si="0"/>
-        <v>AUTOREL_AGTRDY_MSG</v>
+        <f t="shared" si="1"/>
+        <v>AUTOREL_AGTRDY_METHOD</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
-        <f t="shared" si="0"/>
-        <v>DATASCRIPT</v>
+        <f t="shared" si="1"/>
+        <v>AUTOREL_AGTRDY_MSG</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f t="shared" ref="A66:A88" si="1">LEFT(B66,FIND(":",B66)-1)</f>
-        <v>DISABLE_SHADOWJOB</v>
+        <f t="shared" si="1"/>
+        <v>DATASCRIPT</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C66" s="48" t="s">
-        <v>145</v>
+        <v>24</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f t="shared" si="1"/>
-        <v>DISPLAY</v>
+        <f t="shared" ref="A67:A89" si="8">LEFT(B67,FIND(":",B67)-1)</f>
+        <v>DISABLE_SHADOWJOB</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>146</v>
+        <v>54</v>
+      </c>
+      <c r="C67" s="48" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
-        <f t="shared" si="1"/>
-        <v>DONE_TME</v>
+        <f t="shared" si="8"/>
+        <v>DISPLAY</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>457</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f t="shared" si="1"/>
-        <v>EDTFILE</v>
+        <f t="shared" si="8"/>
+        <v>DONE_TME</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>212</v>
+        <v>457</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f t="shared" si="1"/>
-        <v>EXPIRED_RECALL</v>
+        <f t="shared" si="8"/>
+        <v>EDTFILE</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>458</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f t="shared" si="1"/>
-        <v>FCC_DNC_MSG</v>
+        <f t="shared" si="8"/>
+        <v>EXPIRED_RECALL</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>227</v>
+        <v>458</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f t="shared" si="1"/>
-        <v>FCC_OPTOUT_DIGIT</v>
+        <f t="shared" si="8"/>
+        <v>FCC_DNC_MSG</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f t="shared" si="1"/>
-        <v>IDENT</v>
+        <f t="shared" si="8"/>
+        <v>FCC_OPTOUT_DIGIT</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C73" s="47" t="s">
-        <v>235</v>
+        <v>6</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
-        <f t="shared" si="1"/>
-        <v>OUTDATAPOST</v>
+        <f t="shared" si="8"/>
+        <v>IDENT</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>459</v>
+        <v>15</v>
+      </c>
+      <c r="C74" s="47" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
-        <f t="shared" si="1"/>
-        <v>OUTDATAPRE</v>
+        <f t="shared" si="8"/>
+        <v>OUTDATAPOST</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>342</v>
+        <v>459</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
-        <f t="shared" si="1"/>
-        <v>POST_TRANS</v>
+        <f t="shared" si="8"/>
+        <v>OUTDATAPRE</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>131</v>
+        <v>46</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
-        <f t="shared" si="1"/>
-        <v>REL_DIST</v>
+        <f t="shared" si="8"/>
+        <v>POST_TRANS</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C77" s="46" t="s">
-        <v>383</v>
+        <v>65</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
-        <f t="shared" si="1"/>
-        <v>REL_TME</v>
+        <f t="shared" si="8"/>
+        <v>REL_DIST</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>385</v>
+        <v>81</v>
+      </c>
+      <c r="C78" s="46" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
-        <f t="shared" si="1"/>
-        <v>RUNOFCOM</v>
+        <f t="shared" si="8"/>
+        <v>REL_TME</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C79" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
-        <f t="shared" si="1"/>
-        <v>SINGLEEDIT</v>
+        <f t="shared" si="8"/>
+        <v>RUNOFCOM</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>451</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
-        <f t="shared" si="1"/>
-        <v>TESTMODE</v>
+        <f t="shared" si="8"/>
+        <v>SINGLEEDIT</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>153</v>
+        <v>41</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
-        <f t="shared" si="1"/>
-        <v>TESTOPER</v>
+        <f t="shared" si="8"/>
+        <v>TESTMODE</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>450</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
-        <f t="shared" si="1"/>
-        <v>TRANS_CRIT</v>
+        <f t="shared" si="8"/>
+        <v>TESTOPER</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>134</v>
+        <v>79</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
-        <f t="shared" si="1"/>
-        <v>TRANS_MAP</v>
+        <f t="shared" si="8"/>
+        <v>TRANS_CRIT</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C84" s="47" t="s">
-        <v>135</v>
+        <v>66</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
-        <f t="shared" si="1"/>
-        <v>WAITMSG1</v>
+        <f t="shared" si="8"/>
+        <v>TRANS_MAP</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>149</v>
+        <v>67</v>
+      </c>
+      <c r="C85" s="47" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
-        <f t="shared" si="1"/>
-        <v>WAITMSG2</v>
+        <f t="shared" si="8"/>
+        <v>WAITMSG1</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
-        <f t="shared" si="1"/>
-        <v>WAITMSG3</v>
+        <f t="shared" si="8"/>
+        <v>WAITMSG2</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="8"/>
+        <v>WAITMSG3</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="str">
+        <f t="shared" si="8"/>
         <v>WAITMSG4</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C89" s="4" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3308,6 +3322,7 @@
     <sortCondition ref="B62:B88"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4137,32 +4152,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="55" t="s">
         <v>155</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="57" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="54"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="56"/>
+      <c r="D2" s="53"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="54"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="53"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -4179,46 +4194,46 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="52" t="s">
         <v>164</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="57"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="56"/>
+      <c r="D6" s="53"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="57"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="53"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="57"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="56"/>
+      <c r="D8" s="53"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="57"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D9" s="56"/>
+      <c r="D9" s="53"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -4249,54 +4264,54 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="52" t="s">
         <v>174</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="53" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="57"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="56"/>
+      <c r="D13" s="53"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="57"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="D14" s="56"/>
+      <c r="D14" s="53"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="57"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="56"/>
+      <c r="D15" s="53"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="57"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="D16" s="56"/>
+      <c r="D16" s="53"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="57"/>
+      <c r="A17" s="51"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="56"/>
+      <c r="D17" s="53"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
@@ -4467,74 +4482,74 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="51" t="s">
         <v>211</v>
       </c>
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="52" t="s">
         <v>197</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="57"/>
+      <c r="A31" s="51"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="56"/>
+      <c r="D31" s="53"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="57"/>
+      <c r="A32" s="51"/>
+      <c r="B32" s="52"/>
       <c r="C32" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="D32" s="56"/>
+      <c r="D32" s="53"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="B33" s="57" t="s">
+      <c r="B33" s="52" t="s">
         <v>215</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="D33" s="56" t="s">
+      <c r="D33" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="57"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="52"/>
       <c r="C34" s="9"/>
-      <c r="D34" s="56"/>
+      <c r="D34" s="53"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="57"/>
+      <c r="A35" s="51"/>
+      <c r="B35" s="52"/>
       <c r="C35" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="D35" s="56"/>
+      <c r="D35" s="53"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="52"/>
-      <c r="B36" s="57"/>
+      <c r="A36" s="51"/>
+      <c r="B36" s="52"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="56"/>
+      <c r="D36" s="53"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
-      <c r="B37" s="57"/>
+      <c r="A37" s="51"/>
+      <c r="B37" s="52"/>
       <c r="C37" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="D37" s="56"/>
+      <c r="D37" s="53"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
@@ -4631,30 +4646,30 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="52" t="s">
+      <c r="A45" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="B45" s="57"/>
+      <c r="B45" s="52"/>
       <c r="C45" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="D45" s="56" t="s">
+      <c r="D45" s="53" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="52"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="51"/>
+      <c r="B46" s="52"/>
       <c r="C46" s="9"/>
-      <c r="D46" s="56"/>
+      <c r="D46" s="53"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="52"/>
-      <c r="B47" s="57"/>
+      <c r="A47" s="51"/>
+      <c r="B47" s="52"/>
       <c r="C47" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="D47" s="56"/>
+      <c r="D47" s="53"/>
     </row>
     <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
@@ -4727,32 +4742,32 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="52" t="s">
+      <c r="A53" s="51" t="s">
         <v>249</v>
       </c>
-      <c r="B53" s="57" t="s">
+      <c r="B53" s="52" t="s">
         <v>194</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="D53" s="56" t="s">
+      <c r="D53" s="53" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="52"/>
-      <c r="B54" s="57"/>
+      <c r="A54" s="51"/>
+      <c r="B54" s="52"/>
       <c r="C54" s="9"/>
-      <c r="D54" s="56"/>
+      <c r="D54" s="53"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="52"/>
-      <c r="B55" s="57"/>
+      <c r="A55" s="51"/>
+      <c r="B55" s="52"/>
       <c r="C55" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="D55" s="56"/>
+      <c r="D55" s="53"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
@@ -4783,7 +4798,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="52" t="s">
+      <c r="A58" s="51" t="s">
         <v>257</v>
       </c>
       <c r="B58" s="9" t="s">
@@ -4792,151 +4807,151 @@
       <c r="C58" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="D58" s="56" t="s">
+      <c r="D58" s="53" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="52"/>
+      <c r="A59" s="51"/>
       <c r="B59" s="9" t="s">
         <v>259</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="D59" s="56"/>
+      <c r="D59" s="53"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="52"/>
+      <c r="A60" s="51"/>
       <c r="B60" s="9" t="s">
         <v>260</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="D60" s="56"/>
+      <c r="D60" s="53"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="52"/>
+      <c r="A61" s="51"/>
       <c r="B61" s="9" t="s">
         <v>261</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="D61" s="56"/>
+      <c r="D61" s="53"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="52"/>
+      <c r="A62" s="51"/>
       <c r="B62" s="9" t="s">
         <v>262</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="D62" s="56"/>
+      <c r="D62" s="53"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="52"/>
+      <c r="A63" s="51"/>
       <c r="B63" s="9" t="s">
         <v>263</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="D63" s="56"/>
+      <c r="D63" s="53"/>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="52" t="s">
+      <c r="A64" s="51" t="s">
         <v>270</v>
       </c>
-      <c r="B64" s="57" t="s">
+      <c r="B64" s="52" t="s">
         <v>271</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="D64" s="56" t="s">
+      <c r="D64" s="53" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="52"/>
-      <c r="B65" s="57"/>
+      <c r="A65" s="51"/>
+      <c r="B65" s="52"/>
       <c r="C65" s="9"/>
-      <c r="D65" s="56"/>
+      <c r="D65" s="53"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="52"/>
-      <c r="B66" s="57"/>
+      <c r="A66" s="51"/>
+      <c r="B66" s="52"/>
       <c r="C66" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="D66" s="56"/>
+      <c r="D66" s="53"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="52"/>
-      <c r="B67" s="57"/>
+      <c r="A67" s="51"/>
+      <c r="B67" s="52"/>
       <c r="C67" s="10"/>
-      <c r="D67" s="56"/>
+      <c r="D67" s="53"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="52"/>
-      <c r="B68" s="57"/>
+      <c r="A68" s="51"/>
+      <c r="B68" s="52"/>
       <c r="C68" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="D68" s="56"/>
+      <c r="D68" s="53"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="52"/>
-      <c r="B69" s="57"/>
+      <c r="A69" s="51"/>
+      <c r="B69" s="52"/>
       <c r="C69" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="D69" s="56"/>
+      <c r="D69" s="53"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="52"/>
-      <c r="B70" s="57"/>
+      <c r="A70" s="51"/>
+      <c r="B70" s="52"/>
       <c r="C70" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="D70" s="56"/>
+      <c r="D70" s="53"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="52"/>
-      <c r="B71" s="57"/>
+      <c r="A71" s="51"/>
+      <c r="B71" s="52"/>
       <c r="C71" s="9"/>
-      <c r="D71" s="56"/>
+      <c r="D71" s="53"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="52" t="s">
+      <c r="A72" s="51" t="s">
         <v>277</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="C72" s="57" t="s">
+      <c r="C72" s="52" t="s">
         <v>280</v>
       </c>
-      <c r="D72" s="56" t="s">
+      <c r="D72" s="53" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="52"/>
+      <c r="A73" s="51"/>
       <c r="B73" s="9"/>
-      <c r="C73" s="57"/>
-      <c r="D73" s="56"/>
+      <c r="C73" s="52"/>
+      <c r="D73" s="53"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="52"/>
+      <c r="A74" s="51"/>
       <c r="B74" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="C74" s="57"/>
-      <c r="D74" s="56"/>
+      <c r="C74" s="52"/>
+      <c r="D74" s="53"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
@@ -5107,46 +5122,46 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="52" t="s">
+      <c r="A87" s="51" t="s">
         <v>307</v>
       </c>
-      <c r="B87" s="57" t="s">
+      <c r="B87" s="52" t="s">
         <v>194</v>
       </c>
       <c r="C87" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="D87" s="56" t="s">
+      <c r="D87" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="52"/>
-      <c r="B88" s="57"/>
+      <c r="A88" s="51"/>
+      <c r="B88" s="52"/>
       <c r="C88" s="9"/>
-      <c r="D88" s="56"/>
+      <c r="D88" s="53"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="52"/>
-      <c r="B89" s="57"/>
+      <c r="A89" s="51"/>
+      <c r="B89" s="52"/>
       <c r="C89" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="D89" s="56"/>
+      <c r="D89" s="53"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="52"/>
-      <c r="B90" s="57"/>
+      <c r="A90" s="51"/>
+      <c r="B90" s="52"/>
       <c r="C90" s="9"/>
-      <c r="D90" s="56"/>
+      <c r="D90" s="53"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="52"/>
-      <c r="B91" s="57"/>
+      <c r="A91" s="51"/>
+      <c r="B91" s="52"/>
       <c r="C91" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="D91" s="56"/>
+      <c r="D91" s="53"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
@@ -5219,7 +5234,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="52" t="s">
+      <c r="A97" s="51" t="s">
         <v>323</v>
       </c>
       <c r="B97" s="9" t="s">
@@ -5228,25 +5243,25 @@
       <c r="C97" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="D97" s="56" t="s">
+      <c r="D97" s="53" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="52"/>
+      <c r="A98" s="51"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
-      <c r="D98" s="56"/>
+      <c r="D98" s="53"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="52"/>
+      <c r="A99" s="51"/>
       <c r="B99" s="9" t="s">
         <v>325</v>
       </c>
       <c r="C99" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="D99" s="56"/>
+      <c r="D99" s="53"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
@@ -5319,130 +5334,130 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="52" t="s">
+      <c r="A105" s="51" t="s">
         <v>339</v>
       </c>
-      <c r="B105" s="57" t="s">
+      <c r="B105" s="52" t="s">
         <v>194</v>
       </c>
       <c r="C105" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="D105" s="56" t="s">
+      <c r="D105" s="53" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="52"/>
-      <c r="B106" s="57"/>
+      <c r="A106" s="51"/>
+      <c r="B106" s="52"/>
       <c r="C106" s="9"/>
-      <c r="D106" s="56"/>
+      <c r="D106" s="53"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="52"/>
-      <c r="B107" s="57"/>
+      <c r="A107" s="51"/>
+      <c r="B107" s="52"/>
       <c r="C107" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="D107" s="56"/>
+      <c r="D107" s="53"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="52" t="s">
+      <c r="A108" s="51" t="s">
         <v>341</v>
       </c>
-      <c r="B108" s="57" t="s">
+      <c r="B108" s="52" t="s">
         <v>194</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="D108" s="56" t="s">
+      <c r="D108" s="53" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="52"/>
-      <c r="B109" s="57"/>
+      <c r="A109" s="51"/>
+      <c r="B109" s="52"/>
       <c r="C109" s="9"/>
-      <c r="D109" s="56"/>
+      <c r="D109" s="53"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="52"/>
-      <c r="B110" s="57"/>
+      <c r="A110" s="51"/>
+      <c r="B110" s="52"/>
       <c r="C110" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="D110" s="56"/>
+      <c r="D110" s="53"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="52" t="s">
+      <c r="A111" s="51" t="s">
         <v>344</v>
       </c>
-      <c r="B111" s="57" t="s">
+      <c r="B111" s="52" t="s">
         <v>194</v>
       </c>
       <c r="C111" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="D111" s="56" t="s">
+      <c r="D111" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="52"/>
-      <c r="B112" s="57"/>
+      <c r="A112" s="51"/>
+      <c r="B112" s="52"/>
       <c r="C112" s="9"/>
-      <c r="D112" s="56"/>
+      <c r="D112" s="53"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="52"/>
-      <c r="B113" s="57"/>
+      <c r="A113" s="51"/>
+      <c r="B113" s="52"/>
       <c r="C113" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="D113" s="56"/>
+      <c r="D113" s="53"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="52"/>
-      <c r="B114" s="57"/>
+      <c r="A114" s="51"/>
+      <c r="B114" s="52"/>
       <c r="C114" s="9"/>
-      <c r="D114" s="56"/>
+      <c r="D114" s="53"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="52"/>
-      <c r="B115" s="57"/>
+      <c r="A115" s="51"/>
+      <c r="B115" s="52"/>
       <c r="C115" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="D115" s="56"/>
+      <c r="D115" s="53"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="52" t="s">
+      <c r="A116" s="51" t="s">
         <v>348</v>
       </c>
-      <c r="B116" s="57" t="s">
+      <c r="B116" s="52" t="s">
         <v>349</v>
       </c>
       <c r="C116" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="D116" s="56" t="s">
+      <c r="D116" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="52"/>
-      <c r="B117" s="57"/>
+      <c r="A117" s="51"/>
+      <c r="B117" s="52"/>
       <c r="C117" s="9"/>
-      <c r="D117" s="56"/>
+      <c r="D117" s="53"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="52"/>
-      <c r="B118" s="57"/>
+      <c r="A118" s="51"/>
+      <c r="B118" s="52"/>
       <c r="C118" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="D118" s="56"/>
+      <c r="D118" s="53"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
@@ -5712,87 +5727,87 @@
       <c r="A139" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="B139" s="57" t="s">
+      <c r="B139" s="52" t="s">
         <v>194</v>
       </c>
       <c r="C139" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="D139" s="56" t="s">
+      <c r="D139" s="53" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
-      <c r="B140" s="57"/>
+      <c r="B140" s="52"/>
       <c r="C140" s="9"/>
-      <c r="D140" s="56"/>
+      <c r="D140" s="53"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="B141" s="57"/>
+      <c r="B141" s="52"/>
       <c r="C141" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="D141" s="56"/>
+      <c r="D141" s="53"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="52" t="s">
+      <c r="A142" s="51" t="s">
         <v>397</v>
       </c>
-      <c r="B142" s="57" t="s">
+      <c r="B142" s="52" t="s">
         <v>194</v>
       </c>
       <c r="C142" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="D142" s="56" t="s">
+      <c r="D142" s="53" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="52"/>
-      <c r="B143" s="57"/>
+      <c r="A143" s="51"/>
+      <c r="B143" s="52"/>
       <c r="C143" s="9"/>
-      <c r="D143" s="56"/>
+      <c r="D143" s="53"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="52"/>
-      <c r="B144" s="57"/>
+      <c r="A144" s="51"/>
+      <c r="B144" s="52"/>
       <c r="C144" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="D144" s="56"/>
+      <c r="D144" s="53"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="52" t="s">
+      <c r="A145" s="51" t="s">
         <v>400</v>
       </c>
-      <c r="B145" s="57" t="s">
+      <c r="B145" s="52" t="s">
         <v>187</v>
       </c>
       <c r="C145" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="D145" s="56" t="s">
+      <c r="D145" s="53" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="52"/>
-      <c r="B146" s="57"/>
+      <c r="A146" s="51"/>
+      <c r="B146" s="52"/>
       <c r="C146" s="9"/>
-      <c r="D146" s="56"/>
+      <c r="D146" s="53"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="52"/>
-      <c r="B147" s="57"/>
+      <c r="A147" s="51"/>
+      <c r="B147" s="52"/>
       <c r="C147" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="D147" s="56"/>
+      <c r="D147" s="53"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
@@ -5823,32 +5838,32 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="52" t="s">
+      <c r="A150" s="51" t="s">
         <v>407</v>
       </c>
-      <c r="B150" s="57" t="s">
+      <c r="B150" s="52" t="s">
         <v>408</v>
       </c>
       <c r="C150" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="D150" s="56" t="s">
+      <c r="D150" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="52"/>
-      <c r="B151" s="57"/>
+      <c r="A151" s="51"/>
+      <c r="B151" s="52"/>
       <c r="C151" s="9"/>
-      <c r="D151" s="56"/>
+      <c r="D151" s="53"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="52"/>
-      <c r="B152" s="57"/>
+      <c r="A152" s="51"/>
+      <c r="B152" s="52"/>
       <c r="C152" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="D152" s="56"/>
+      <c r="D152" s="53"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
@@ -5865,60 +5880,60 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="52" t="s">
+      <c r="A154" s="51" t="s">
         <v>413</v>
       </c>
       <c r="B154" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="C154" s="57" t="s">
+      <c r="C154" s="52" t="s">
         <v>416</v>
       </c>
-      <c r="D154" s="56" t="s">
+      <c r="D154" s="53" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="52"/>
+      <c r="A155" s="51"/>
       <c r="B155" s="9"/>
-      <c r="C155" s="57"/>
-      <c r="D155" s="56"/>
+      <c r="C155" s="52"/>
+      <c r="D155" s="53"/>
     </row>
     <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A156" s="52"/>
+      <c r="A156" s="51"/>
       <c r="B156" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="C156" s="57"/>
-      <c r="D156" s="56"/>
+      <c r="C156" s="52"/>
+      <c r="D156" s="53"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="52" t="s">
+      <c r="A157" s="51" t="s">
         <v>417</v>
       </c>
       <c r="B157" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="C157" s="57" t="s">
+      <c r="C157" s="52" t="s">
         <v>420</v>
       </c>
-      <c r="D157" s="56" t="s">
+      <c r="D157" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="52"/>
+      <c r="A158" s="51"/>
       <c r="B158" s="9"/>
-      <c r="C158" s="57"/>
-      <c r="D158" s="56"/>
+      <c r="C158" s="52"/>
+      <c r="D158" s="53"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="52"/>
+      <c r="A159" s="51"/>
       <c r="B159" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="C159" s="57"/>
-      <c r="D159" s="56"/>
+      <c r="C159" s="52"/>
+      <c r="D159" s="53"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
@@ -5949,7 +5964,7 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="52" t="s">
+      <c r="A162" s="51" t="s">
         <v>425</v>
       </c>
       <c r="B162" s="9" t="s">
@@ -5958,53 +5973,53 @@
       <c r="C162" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="D162" s="56" t="s">
+      <c r="D162" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="52"/>
+      <c r="A163" s="51"/>
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
-      <c r="D163" s="56"/>
+      <c r="D163" s="53"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="52"/>
+      <c r="A164" s="51"/>
       <c r="B164" s="9" t="s">
         <v>427</v>
       </c>
       <c r="C164" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="D164" s="56"/>
+      <c r="D164" s="53"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="52"/>
+      <c r="A165" s="51"/>
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
-      <c r="D165" s="56"/>
+      <c r="D165" s="53"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="52"/>
+      <c r="A166" s="51"/>
       <c r="B166" s="9" t="s">
         <v>428</v>
       </c>
       <c r="C166" s="9"/>
-      <c r="D166" s="56"/>
+      <c r="D166" s="53"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="52"/>
+      <c r="A167" s="51"/>
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
-      <c r="D167" s="56"/>
+      <c r="D167" s="53"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="52"/>
+      <c r="A168" s="51"/>
       <c r="B168" s="9" t="s">
         <v>429</v>
       </c>
       <c r="C168" s="9"/>
-      <c r="D168" s="56"/>
+      <c r="D168" s="53"/>
     </row>
     <row r="169" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
@@ -6035,46 +6050,46 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="52" t="s">
+      <c r="A171" s="51" t="s">
         <v>436</v>
       </c>
       <c r="B171" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="C171" s="57" t="s">
+      <c r="C171" s="52" t="s">
         <v>438</v>
       </c>
-      <c r="D171" s="56" t="s">
+      <c r="D171" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="52"/>
+      <c r="A172" s="51"/>
       <c r="B172" s="9"/>
-      <c r="C172" s="57"/>
-      <c r="D172" s="56"/>
+      <c r="C172" s="52"/>
+      <c r="D172" s="53"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="52"/>
+      <c r="A173" s="51"/>
       <c r="B173" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="C173" s="57"/>
-      <c r="D173" s="56"/>
+      <c r="C173" s="52"/>
+      <c r="D173" s="53"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="52"/>
+      <c r="A174" s="51"/>
       <c r="B174" s="9"/>
-      <c r="C174" s="57"/>
-      <c r="D174" s="56"/>
+      <c r="C174" s="52"/>
+      <c r="D174" s="53"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="52"/>
+      <c r="A175" s="51"/>
       <c r="B175" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="C175" s="57"/>
-      <c r="D175" s="56"/>
+      <c r="C175" s="52"/>
+      <c r="D175" s="53"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="12" t="s">
@@ -6105,46 +6120,46 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="52" t="s">
+      <c r="A178" s="51" t="s">
         <v>443</v>
       </c>
-      <c r="B178" s="57" t="s">
+      <c r="B178" s="52" t="s">
         <v>444</v>
       </c>
       <c r="C178" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D178" s="56" t="s">
+      <c r="D178" s="53" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="52"/>
-      <c r="B179" s="57"/>
+      <c r="A179" s="51"/>
+      <c r="B179" s="52"/>
       <c r="C179" s="9"/>
-      <c r="D179" s="56"/>
+      <c r="D179" s="53"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="52"/>
-      <c r="B180" s="57"/>
+      <c r="A180" s="51"/>
+      <c r="B180" s="52"/>
       <c r="C180" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="D180" s="56"/>
+      <c r="D180" s="53"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="52"/>
-      <c r="B181" s="57"/>
+      <c r="A181" s="51"/>
+      <c r="B181" s="52"/>
       <c r="C181" s="9"/>
-      <c r="D181" s="56"/>
+      <c r="D181" s="53"/>
     </row>
     <row r="182" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A182" s="52"/>
-      <c r="B182" s="57"/>
+      <c r="A182" s="51"/>
+      <c r="B182" s="52"/>
       <c r="C182" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="D182" s="56"/>
+      <c r="D182" s="53"/>
     </row>
     <row r="183" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="14" t="s">
@@ -6163,6 +6178,63 @@
     <row r="184" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="D12:D17"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="A64:A71"/>
+    <mergeCell ref="B64:B71"/>
+    <mergeCell ref="D64:D71"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="D33:D37"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="A58:A63"/>
+    <mergeCell ref="D58:D63"/>
+    <mergeCell ref="A105:A107"/>
+    <mergeCell ref="B105:B107"/>
+    <mergeCell ref="D105:D107"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="D72:D74"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="D87:D91"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="D97:D99"/>
+    <mergeCell ref="A142:A144"/>
+    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="D142:D144"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="D108:D110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="B111:B115"/>
+    <mergeCell ref="D111:D115"/>
+    <mergeCell ref="A116:A118"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="D116:D118"/>
+    <mergeCell ref="B139:B141"/>
+    <mergeCell ref="D139:D141"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="B145:B147"/>
+    <mergeCell ref="D145:D147"/>
+    <mergeCell ref="A150:A152"/>
+    <mergeCell ref="B150:B152"/>
+    <mergeCell ref="D150:D152"/>
     <mergeCell ref="A178:A182"/>
     <mergeCell ref="B178:B182"/>
     <mergeCell ref="D178:D182"/>
@@ -6177,63 +6249,6 @@
     <mergeCell ref="A171:A175"/>
     <mergeCell ref="C171:C175"/>
     <mergeCell ref="D171:D175"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="B145:B147"/>
-    <mergeCell ref="D145:D147"/>
-    <mergeCell ref="A150:A152"/>
-    <mergeCell ref="B150:B152"/>
-    <mergeCell ref="D150:D152"/>
-    <mergeCell ref="A142:A144"/>
-    <mergeCell ref="B142:B144"/>
-    <mergeCell ref="D142:D144"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="D108:D110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="B111:B115"/>
-    <mergeCell ref="D111:D115"/>
-    <mergeCell ref="A116:A118"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="D116:D118"/>
-    <mergeCell ref="B139:B141"/>
-    <mergeCell ref="D139:D141"/>
-    <mergeCell ref="A105:A107"/>
-    <mergeCell ref="B105:B107"/>
-    <mergeCell ref="D105:D107"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="D72:D74"/>
-    <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="D87:D91"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="D97:D99"/>
-    <mergeCell ref="A64:A71"/>
-    <mergeCell ref="B64:B71"/>
-    <mergeCell ref="D64:D71"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="D33:D37"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="A58:A63"/>
-    <mergeCell ref="D58:D63"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="D12:D17"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="D5:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
02.10.2017 add headers tag &  ovewview
</commit_message>
<xml_diff>
--- a/Job_template.xlsx
+++ b/Job_template.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -12,7 +12,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId3"/>
     <sheet name="Sections" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="540">
   <si>
     <t>EDTFILE:outbound:</t>
   </si>
@@ -1507,11 +1507,207 @@
   <si>
     <t>Automatically start Update mode on customer hang up</t>
   </si>
+  <si>
+    <t>JLABEL</t>
+  </si>
+  <si>
+    <t>PORTS</t>
+  </si>
+  <si>
+    <t>ANI_FIELD</t>
+  </si>
+  <si>
+    <t>AUTOCALLSEL_TRIGGER</t>
+  </si>
+  <si>
+    <t>LOGONUNIT</t>
+  </si>
+  <si>
+    <t>TRANSID</t>
+  </si>
+  <si>
+    <t>TRANSTAT</t>
+  </si>
+  <si>
+    <t>HITRATE</t>
+  </si>
+  <si>
+    <t>IDMODE</t>
+  </si>
+  <si>
+    <t>MINHITRATE</t>
+  </si>
+  <si>
+    <t>ECPA</t>
+  </si>
+  <si>
+    <t>LIST</t>
+  </si>
+  <si>
+    <t>OKEYS</t>
+  </si>
+  <si>
+    <t>SCREEN</t>
+  </si>
+  <si>
+    <t>TRANSFER_TO_JOB</t>
+  </si>
+  <si>
+    <t>TRANJOB</t>
+  </si>
+  <si>
+    <t>VIRTUAL</t>
+  </si>
+  <si>
+    <t>OFCOM</t>
+  </si>
+  <si>
+    <t>OFCOM_METHOD</t>
+  </si>
+  <si>
+    <t>DATAPROCESS</t>
+  </si>
+  <si>
+    <t>PVDIAL</t>
+  </si>
+  <si>
+    <t>PVCANCEL</t>
+  </si>
+  <si>
+    <t>PVLENGTH</t>
+  </si>
+  <si>
+    <t>PVSEARCHTYPE</t>
+  </si>
+  <si>
+    <t>JOBEND</t>
+  </si>
+  <si>
+    <t>MAKE_CALL_VDN</t>
+  </si>
+  <si>
+    <t>ORDERZONES</t>
+  </si>
+  <si>
+    <t>POSTUPDATE</t>
+  </si>
+  <si>
+    <t>RECALL_CPA</t>
+  </si>
+  <si>
+    <t>OFCOMTIMER</t>
+  </si>
+  <si>
+    <t>OFCOMFR</t>
+  </si>
+  <si>
+    <t>WAITLIMIT</t>
+  </si>
+  <si>
+    <t>XFERHOLDMSGNO</t>
+  </si>
+  <si>
+    <t>AUTOEND</t>
+  </si>
+  <si>
+    <t>DATASCRIPT</t>
+  </si>
+  <si>
+    <t>DONE_TME</t>
+  </si>
+  <si>
+    <t>EDTFILE</t>
+  </si>
+  <si>
+    <t>IDENT</t>
+  </si>
+  <si>
+    <t>OUTDATAPRE</t>
+  </si>
+  <si>
+    <t>POST_TRANS</t>
+  </si>
+  <si>
+    <t>REL_DIST</t>
+  </si>
+  <si>
+    <t>REL_TME</t>
+  </si>
+  <si>
+    <t>RUNOFCOM</t>
+  </si>
+  <si>
+    <t>TESTMODE</t>
+  </si>
+  <si>
+    <t>TESTOPER</t>
+  </si>
+  <si>
+    <t>TRANS_CRIT</t>
+  </si>
+  <si>
+    <t>TRANS_MAP</t>
+  </si>
+  <si>
+    <t>WAITMSG1</t>
+  </si>
+  <si>
+    <t>WAITMSG2</t>
+  </si>
+  <si>
+    <t>WAITMSG3</t>
+  </si>
+  <si>
+    <t>WAITMSG4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E - Expert Calling Ratio   C - Cruise Control </t>
+  </si>
+  <si>
+    <r>
+      <t>Call Pacing method</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Transaction verification job</t>
+  </si>
+  <si>
+    <t>. YES = Job uses sales verification</t>
+  </si>
+  <si>
+    <t>Expert calling ratio (intelligent dialing mode)</t>
+  </si>
+  <si>
+    <t>Job name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The default is usually NO, with no ability to edit on the Job Verification screen.</t>
+  </si>
+  <si>
+    <t>YES = Allow only single edit of field in agent input.</t>
+  </si>
+  <si>
+    <t>Number of seconds agents are allowed for talk time (talktime) and update time (updtime)</t>
+  </si>
+  <si>
+    <t>Message to the called party after the called party opts out to DNC.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1670,7 +1866,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1784,20 +1980,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1849,7 +2036,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1861,7 +2047,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2167,7 +2352,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2175,1152 +2360,808 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="114.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="78.7109375" customWidth="1"/>
+    <col min="3" max="3" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="str">
-        <f t="shared" ref="A2:A5" si="0">LEFT(B2,FIND(":",B2)-1)</f>
-        <v>JLABEL</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="37" t="s">
+      <c r="B1" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>STARTTIME</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="6" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>407</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>STOPTIME</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>PORTS</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="6" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="str">
-        <f>LEFT(B6,FIND(":",B6)-1)</f>
-        <v>ANI</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D6">
-        <f>FIND("I",B6)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="str">
-        <f t="shared" ref="A7:A66" si="1">LEFT(B7,FIND(":",B7)-1)</f>
-        <v>ANI_FIELD</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>481</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>AUTOCALLSEL_TRIGGER</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>LOGONUNIT</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="37" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>TRANSID</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>484</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>TRANSTAT</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v>CPMETHOD</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v>HITRATE</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="6" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C12" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>486</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v>IDMODE</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="3" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>487</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="C14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v>MINHITRATE</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>488</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="str">
-        <f t="shared" ref="A16:A18" si="2">LEFT(B16,FIND(":",B16)-1)</f>
-        <v>ECPA</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v>LIST</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="1" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>490</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v>SELECT</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="1" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="str">
-        <f t="shared" si="1"/>
-        <v>DNC_GROUP</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="str">
-        <f t="shared" si="1"/>
-        <v>OKEYS</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="1" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>491</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="str">
-        <f t="shared" si="1"/>
-        <v>SCREEN</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="1" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>492</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="str">
-        <f t="shared" si="1"/>
-        <v>TRANSFER_TO_JOB</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="1" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>493</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="str">
-        <f t="shared" ref="A23" si="3">LEFT(B23,FIND(":",B23)-1)</f>
-        <v>OKEYS</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="1" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>491</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>IVR_AGENTS</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="1" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="D24" s="22"/>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>IVR_ID</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="1" t="s">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="D25" s="22"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>IVR_INITSCRIPT</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="1" t="s">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="D26" s="22"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="str">
-        <f t="shared" si="1"/>
-        <v>IVR_SCRIPT</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="1" t="s">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="D27" s="22"/>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="str">
-        <f t="shared" ref="A28" si="4">LEFT(B28,FIND(":",B28)-1)</f>
-        <v>TRANJOB</v>
-      </c>
-      <c r="B28" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>136</v>
-      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>494</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C28" t="s">
+        <v>533</v>
+      </c>
+      <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="str">
-        <f t="shared" ref="A29" si="5">LEFT(B29,FIND(":",B29)-1)</f>
-        <v>VIRTUAL</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="1" t="s">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>495</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v>OFCOM</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="1" t="s">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>496</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="D30" s="22"/>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="str">
-        <f t="shared" si="1"/>
-        <v>OFCOM_METHOD</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="str">
-        <f t="shared" ref="A32:A33" si="6">LEFT(B32,FIND(":",B32)-1)</f>
-        <v>FCC</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="1" t="s">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>497</v>
+      </c>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="D32" s="22"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="str">
-        <f t="shared" si="6"/>
-        <v>RUNCALL</v>
-      </c>
-      <c r="B33" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="1" t="s">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
+        <v>391</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="D33" s="22"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>DATAPROCESS</v>
-      </c>
-      <c r="B34" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="6" t="s">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="34" t="s">
+        <v>498</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="D34" s="22"/>
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="38" t="str">
-        <f t="shared" ref="A35" si="7">LEFT(B35,FIND(":",B35)-1)</f>
-        <v>PVDIAL</v>
-      </c>
-      <c r="B35" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="45" t="s">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
+        <v>499</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="D35" s="22"/>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>PVCANCEL</v>
-      </c>
-      <c r="B36" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="1" t="s">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="37" t="s">
+        <v>500</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="D36" s="22"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>PVEMPTYREC</v>
-      </c>
-      <c r="B37" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="1" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="37" t="s">
+        <v>358</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="D37" s="22"/>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>PVIGNOREDEL</v>
-      </c>
-      <c r="B38" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="6" t="s">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="37" t="s">
+        <v>360</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="D38" s="22"/>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>PVKEYFLD</v>
-      </c>
-      <c r="B39" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="1" t="s">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="s">
+        <v>362</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>PVLENGTH</v>
-      </c>
-      <c r="B40" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="1" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="37" t="s">
+        <v>501</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="str">
-        <f t="shared" si="1"/>
-        <v>PVSEARCHTYPE</v>
-      </c>
-      <c r="B41" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" s="1" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="37" t="s">
+        <v>502</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="str">
-        <f t="shared" si="1"/>
-        <v>JOBEND</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="1" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="39" t="s">
+        <v>503</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="40" t="str">
-        <f t="shared" si="1"/>
-        <v>LOWALTQPRIO</v>
-      </c>
-      <c r="B43" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="7" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="39" t="s">
+        <v>303</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="40" t="str">
-        <f t="shared" si="1"/>
-        <v>MAKE_CALL_VDN</v>
-      </c>
-      <c r="B44" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="1" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="39" t="s">
+        <v>504</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="40" t="str">
-        <f t="shared" si="1"/>
-        <v>ORDERZONES</v>
-      </c>
-      <c r="B45" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="1" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="39" t="s">
+        <v>505</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v>AUTORELEASE</v>
-      </c>
-      <c r="B46" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" s="7" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v>POSTUPDATE</v>
-      </c>
-      <c r="B47" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="1" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="43" t="s">
+        <v>506</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>QUOTA_EXTFILE</v>
-      </c>
-      <c r="B48" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C48" s="1" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="41" t="s">
+        <v>371</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>QUOTA_SAVE</v>
-      </c>
-      <c r="B49" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="C49" s="1" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="41" t="s">
+        <v>373</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>QUOTAVAL</v>
-      </c>
-      <c r="B50" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" s="1" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="41" t="s">
+        <v>369</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>INF_ESC_RECALL</v>
-      </c>
-      <c r="B51" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" s="1" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>INF_RECALL_GETOP_JOB</v>
-      </c>
-      <c r="B52" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C52" s="1" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>RECALL_CPA</v>
-      </c>
-      <c r="B53" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="C53" s="1" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>507</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>RECALL_INTERVAL</v>
-      </c>
-      <c r="B54" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" s="1" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>RECALL_NOTIFY</v>
-      </c>
-      <c r="B55" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" s="1" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>RECALL_NUMOFTRY</v>
-      </c>
-      <c r="B56" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C56" s="1" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="34" t="str">
-        <f t="shared" si="1"/>
-        <v>OFCOMTIMER</v>
-      </c>
-      <c r="B57" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="1" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="33" t="s">
+        <v>508</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="D57" s="22"/>
       <c r="E57" s="22"/>
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
-      <c r="H57" s="22"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="34" t="str">
-        <f t="shared" si="1"/>
-        <v>OFCOMFR</v>
-      </c>
-      <c r="B58" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C58" s="1" t="s">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
+        <v>509</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="34" t="str">
-        <f t="shared" si="1"/>
-        <v>CONNTOLE</v>
-      </c>
-      <c r="B59" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="8" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="34" t="str">
-        <f t="shared" si="1"/>
-        <v>SERVICELEVEL</v>
-      </c>
-      <c r="B60" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C60" s="7" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="50" t="str">
-        <f t="shared" si="1"/>
-        <v>WAITLIMIT</v>
-      </c>
-      <c r="B61" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="C61" s="1" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="48" t="s">
+        <v>510</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="50" t="str">
-        <f t="shared" si="1"/>
-        <v>XFERHOLDMSGNO</v>
-      </c>
-      <c r="B62" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="C62" s="47" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="48" t="s">
+        <v>511</v>
+      </c>
+      <c r="B62" s="45" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="37" t="str">
-        <f t="shared" si="1"/>
-        <v>AUTOEND</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C63" s="4" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>512</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="str">
-        <f t="shared" si="1"/>
-        <v>AUTOREL_AGTRDY_METHOD</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C64" s="4" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>173</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="str">
-        <f t="shared" si="1"/>
-        <v>AUTOREL_AGTRDY_MSG</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C65" s="4" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>180</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="str">
-        <f t="shared" si="1"/>
-        <v>DATASCRIPT</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C66" s="4" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>513</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="str">
-        <f t="shared" ref="A67:A89" si="8">LEFT(B67,FIND(":",B67)-1)</f>
-        <v>DISABLE_SHADOWJOB</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C67" s="48" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>201</v>
+      </c>
+      <c r="B67" s="46" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="str">
-        <f t="shared" si="8"/>
-        <v>DISPLAY</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C68" s="4" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>204</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="str">
-        <f t="shared" si="8"/>
-        <v>DONE_TME</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C69" s="4" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>514</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="str">
-        <f t="shared" si="8"/>
-        <v>EDTFILE</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C70" s="4" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>515</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="str">
-        <f t="shared" si="8"/>
-        <v>EXPIRED_RECALL</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C71" s="4" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>219</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="str">
-        <f t="shared" si="8"/>
-        <v>FCC_DNC_MSG</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="str">
-        <f t="shared" si="8"/>
-        <v>FCC_OPTOUT_DIGIT</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73" s="4" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>226</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>223</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="str">
-        <f t="shared" si="8"/>
-        <v>IDENT</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" s="47" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>516</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="str">
-        <f t="shared" si="8"/>
-        <v>OUTDATAPOST</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C75" s="4" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>339</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="str">
-        <f t="shared" si="8"/>
-        <v>OUTDATAPRE</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C76" s="4" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>517</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="str">
-        <f t="shared" si="8"/>
-        <v>POST_TRANS</v>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>518</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C77" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="str">
-        <f t="shared" si="8"/>
-        <v>REL_DIST</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C78" s="46" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>519</v>
+      </c>
+      <c r="B78" s="44" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="str">
-        <f t="shared" si="8"/>
-        <v>REL_TME</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C79" s="4" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>520</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="str">
-        <f t="shared" si="8"/>
-        <v>RUNOFCOM</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C80" s="1"/>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>521</v>
+      </c>
+      <c r="B80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="str">
-        <f t="shared" si="8"/>
-        <v>SINGLEEDIT</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>451</v>
+      <c r="A81" t="s">
+        <v>405</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="C81" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="str">
-        <f t="shared" si="8"/>
-        <v>TESTMODE</v>
+      <c r="A82" t="s">
+        <v>522</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C82" s="1" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="str">
-        <f t="shared" si="8"/>
-        <v>TESTOPER</v>
+      <c r="A83" t="s">
+        <v>523</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>450</v>
+        <v>538</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="str">
-        <f t="shared" si="8"/>
-        <v>TRANS_CRIT</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C84" s="4" t="s">
+      <c r="A84" t="s">
+        <v>524</v>
+      </c>
+      <c r="B84" s="4" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="str">
-        <f t="shared" si="8"/>
-        <v>TRANS_MAP</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C85" s="47" t="s">
+      <c r="A85" t="s">
+        <v>525</v>
+      </c>
+      <c r="B85" s="4" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="str">
-        <f t="shared" si="8"/>
-        <v>WAITMSG1</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C86" s="5" t="s">
+      <c r="A86" t="s">
+        <v>526</v>
+      </c>
+      <c r="B86" s="4" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="str">
-        <f t="shared" si="8"/>
-        <v>WAITMSG2</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C87" s="5" t="s">
+      <c r="A87" t="s">
+        <v>527</v>
+      </c>
+      <c r="B87" s="4" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="str">
-        <f t="shared" si="8"/>
-        <v>WAITMSG3</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C88" s="5" t="s">
+      <c r="A88" t="s">
+        <v>528</v>
+      </c>
+      <c r="B88" s="4" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="str">
-        <f t="shared" si="8"/>
-        <v>WAITMSG4</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C89" s="4" t="s">
+      <c r="A89" t="s">
+        <v>529</v>
+      </c>
+      <c r="B89" s="4" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B62:C88">
-    <sortCondition ref="B62:B88"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3330,7 +3171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -4139,8 +3980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D184"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4152,32 +3993,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="53" t="s">
         <v>155</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="55" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="54"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="53"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
-      <c r="B3" s="56"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -4194,46 +4035,46 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="50" t="s">
         <v>164</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="53"/>
+      <c r="D6" s="51"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
-      <c r="B7" s="52"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D7" s="53"/>
+      <c r="D7" s="51"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="52"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="53"/>
+      <c r="D8" s="51"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D9" s="53"/>
+      <c r="D9" s="51"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -4264,54 +4105,54 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="49" t="s">
         <v>173</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="50" t="s">
         <v>174</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="51" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
-      <c r="B13" s="52"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="53"/>
+      <c r="D13" s="51"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="D14" s="53"/>
+      <c r="D14" s="51"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="D15" s="53"/>
+      <c r="D15" s="51"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="D16" s="53"/>
+      <c r="D16" s="51"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="53"/>
+      <c r="D17" s="51"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
@@ -4482,74 +4323,74 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="49" t="s">
         <v>211</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="50" t="s">
         <v>197</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D30" s="53" t="s">
+      <c r="D30" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="51"/>
-      <c r="B31" s="52"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="50"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="53"/>
+      <c r="D31" s="51"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="51"/>
-      <c r="B32" s="52"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="50"/>
       <c r="C32" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="D32" s="53"/>
+      <c r="D32" s="51"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="50" t="s">
         <v>215</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="D33" s="53" t="s">
+      <c r="D33" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="51"/>
-      <c r="B34" s="52"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="9"/>
-      <c r="D34" s="53"/>
+      <c r="D34" s="51"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="51"/>
-      <c r="B35" s="52"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="50"/>
       <c r="C35" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="D35" s="53"/>
+      <c r="D35" s="51"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="51"/>
-      <c r="B36" s="52"/>
+      <c r="A36" s="49"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="53"/>
+      <c r="D36" s="51"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="51"/>
-      <c r="B37" s="52"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="D37" s="53"/>
+      <c r="D37" s="51"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
@@ -4646,30 +4487,30 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="B45" s="52"/>
+      <c r="B45" s="50"/>
       <c r="C45" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="D45" s="53" t="s">
+      <c r="D45" s="51" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="51"/>
-      <c r="B46" s="52"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="50"/>
       <c r="C46" s="9"/>
-      <c r="D46" s="53"/>
+      <c r="D46" s="51"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="51"/>
-      <c r="B47" s="52"/>
+      <c r="A47" s="49"/>
+      <c r="B47" s="50"/>
       <c r="C47" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="D47" s="53"/>
+      <c r="D47" s="51"/>
     </row>
     <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
@@ -4742,32 +4583,32 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="51" t="s">
+      <c r="A53" s="49" t="s">
         <v>249</v>
       </c>
-      <c r="B53" s="52" t="s">
+      <c r="B53" s="50" t="s">
         <v>194</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="D53" s="53" t="s">
+      <c r="D53" s="51" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="51"/>
-      <c r="B54" s="52"/>
+      <c r="A54" s="49"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="9"/>
-      <c r="D54" s="53"/>
+      <c r="D54" s="51"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="51"/>
-      <c r="B55" s="52"/>
+      <c r="A55" s="49"/>
+      <c r="B55" s="50"/>
       <c r="C55" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="D55" s="53"/>
+      <c r="D55" s="51"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
@@ -4798,7 +4639,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="51" t="s">
+      <c r="A58" s="49" t="s">
         <v>257</v>
       </c>
       <c r="B58" s="9" t="s">
@@ -4807,151 +4648,151 @@
       <c r="C58" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="D58" s="53" t="s">
+      <c r="D58" s="51" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="51"/>
+      <c r="A59" s="49"/>
       <c r="B59" s="9" t="s">
         <v>259</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="D59" s="53"/>
+      <c r="D59" s="51"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="51"/>
+      <c r="A60" s="49"/>
       <c r="B60" s="9" t="s">
         <v>260</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="D60" s="53"/>
+      <c r="D60" s="51"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="51"/>
+      <c r="A61" s="49"/>
       <c r="B61" s="9" t="s">
         <v>261</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="D61" s="53"/>
+      <c r="D61" s="51"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="51"/>
+      <c r="A62" s="49"/>
       <c r="B62" s="9" t="s">
         <v>262</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="D62" s="53"/>
+      <c r="D62" s="51"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="51"/>
+      <c r="A63" s="49"/>
       <c r="B63" s="9" t="s">
         <v>263</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="D63" s="53"/>
+      <c r="D63" s="51"/>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="51" t="s">
+      <c r="A64" s="49" t="s">
         <v>270</v>
       </c>
-      <c r="B64" s="52" t="s">
+      <c r="B64" s="50" t="s">
         <v>271</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="D64" s="53" t="s">
+      <c r="D64" s="51" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="51"/>
-      <c r="B65" s="52"/>
+      <c r="A65" s="49"/>
+      <c r="B65" s="50"/>
       <c r="C65" s="9"/>
-      <c r="D65" s="53"/>
+      <c r="D65" s="51"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="51"/>
-      <c r="B66" s="52"/>
+      <c r="A66" s="49"/>
+      <c r="B66" s="50"/>
       <c r="C66" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="D66" s="53"/>
+      <c r="D66" s="51"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="51"/>
-      <c r="B67" s="52"/>
+      <c r="A67" s="49"/>
+      <c r="B67" s="50"/>
       <c r="C67" s="10"/>
-      <c r="D67" s="53"/>
+      <c r="D67" s="51"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="51"/>
-      <c r="B68" s="52"/>
+      <c r="A68" s="49"/>
+      <c r="B68" s="50"/>
       <c r="C68" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="D68" s="53"/>
+      <c r="D68" s="51"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="51"/>
-      <c r="B69" s="52"/>
+      <c r="A69" s="49"/>
+      <c r="B69" s="50"/>
       <c r="C69" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="D69" s="53"/>
+      <c r="D69" s="51"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="51"/>
-      <c r="B70" s="52"/>
+      <c r="A70" s="49"/>
+      <c r="B70" s="50"/>
       <c r="C70" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="D70" s="53"/>
+      <c r="D70" s="51"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="51"/>
-      <c r="B71" s="52"/>
+      <c r="A71" s="49"/>
+      <c r="B71" s="50"/>
       <c r="C71" s="9"/>
-      <c r="D71" s="53"/>
+      <c r="D71" s="51"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="51" t="s">
+      <c r="A72" s="49" t="s">
         <v>277</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="C72" s="52" t="s">
+      <c r="C72" s="50" t="s">
         <v>280</v>
       </c>
-      <c r="D72" s="53" t="s">
+      <c r="D72" s="51" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="51"/>
+      <c r="A73" s="49"/>
       <c r="B73" s="9"/>
-      <c r="C73" s="52"/>
-      <c r="D73" s="53"/>
+      <c r="C73" s="50"/>
+      <c r="D73" s="51"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="51"/>
+      <c r="A74" s="49"/>
       <c r="B74" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="C74" s="52"/>
-      <c r="D74" s="53"/>
+      <c r="C74" s="50"/>
+      <c r="D74" s="51"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
@@ -5122,46 +4963,46 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="51" t="s">
+      <c r="A87" s="49" t="s">
         <v>307</v>
       </c>
-      <c r="B87" s="52" t="s">
+      <c r="B87" s="50" t="s">
         <v>194</v>
       </c>
       <c r="C87" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="D87" s="53" t="s">
+      <c r="D87" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="51"/>
-      <c r="B88" s="52"/>
+      <c r="A88" s="49"/>
+      <c r="B88" s="50"/>
       <c r="C88" s="9"/>
-      <c r="D88" s="53"/>
+      <c r="D88" s="51"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="51"/>
-      <c r="B89" s="52"/>
+      <c r="A89" s="49"/>
+      <c r="B89" s="50"/>
       <c r="C89" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="D89" s="53"/>
+      <c r="D89" s="51"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="51"/>
-      <c r="B90" s="52"/>
+      <c r="A90" s="49"/>
+      <c r="B90" s="50"/>
       <c r="C90" s="9"/>
-      <c r="D90" s="53"/>
+      <c r="D90" s="51"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="51"/>
-      <c r="B91" s="52"/>
+      <c r="A91" s="49"/>
+      <c r="B91" s="50"/>
       <c r="C91" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="D91" s="53"/>
+      <c r="D91" s="51"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
@@ -5234,7 +5075,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="51" t="s">
+      <c r="A97" s="49" t="s">
         <v>323</v>
       </c>
       <c r="B97" s="9" t="s">
@@ -5243,25 +5084,25 @@
       <c r="C97" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="D97" s="53" t="s">
+      <c r="D97" s="51" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="51"/>
+      <c r="A98" s="49"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
-      <c r="D98" s="53"/>
+      <c r="D98" s="51"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="51"/>
+      <c r="A99" s="49"/>
       <c r="B99" s="9" t="s">
         <v>325</v>
       </c>
       <c r="C99" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="D99" s="53"/>
+      <c r="D99" s="51"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
@@ -5334,130 +5175,130 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="51" t="s">
+      <c r="A105" s="49" t="s">
         <v>339</v>
       </c>
-      <c r="B105" s="52" t="s">
+      <c r="B105" s="50" t="s">
         <v>194</v>
       </c>
       <c r="C105" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="D105" s="53" t="s">
+      <c r="D105" s="51" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="51"/>
-      <c r="B106" s="52"/>
+      <c r="A106" s="49"/>
+      <c r="B106" s="50"/>
       <c r="C106" s="9"/>
-      <c r="D106" s="53"/>
+      <c r="D106" s="51"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="51"/>
-      <c r="B107" s="52"/>
+      <c r="A107" s="49"/>
+      <c r="B107" s="50"/>
       <c r="C107" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="D107" s="53"/>
+      <c r="D107" s="51"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="51" t="s">
+      <c r="A108" s="49" t="s">
         <v>341</v>
       </c>
-      <c r="B108" s="52" t="s">
+      <c r="B108" s="50" t="s">
         <v>194</v>
       </c>
       <c r="C108" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="D108" s="53" t="s">
+      <c r="D108" s="51" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="51"/>
-      <c r="B109" s="52"/>
+      <c r="A109" s="49"/>
+      <c r="B109" s="50"/>
       <c r="C109" s="9"/>
-      <c r="D109" s="53"/>
+      <c r="D109" s="51"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="51"/>
-      <c r="B110" s="52"/>
+      <c r="A110" s="49"/>
+      <c r="B110" s="50"/>
       <c r="C110" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="D110" s="53"/>
+      <c r="D110" s="51"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="51" t="s">
+      <c r="A111" s="49" t="s">
         <v>344</v>
       </c>
-      <c r="B111" s="52" t="s">
+      <c r="B111" s="50" t="s">
         <v>194</v>
       </c>
       <c r="C111" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="D111" s="53" t="s">
+      <c r="D111" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="51"/>
-      <c r="B112" s="52"/>
+      <c r="A112" s="49"/>
+      <c r="B112" s="50"/>
       <c r="C112" s="9"/>
-      <c r="D112" s="53"/>
+      <c r="D112" s="51"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="51"/>
-      <c r="B113" s="52"/>
+      <c r="A113" s="49"/>
+      <c r="B113" s="50"/>
       <c r="C113" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="D113" s="53"/>
+      <c r="D113" s="51"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="51"/>
-      <c r="B114" s="52"/>
+      <c r="A114" s="49"/>
+      <c r="B114" s="50"/>
       <c r="C114" s="9"/>
-      <c r="D114" s="53"/>
+      <c r="D114" s="51"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="51"/>
-      <c r="B115" s="52"/>
+      <c r="A115" s="49"/>
+      <c r="B115" s="50"/>
       <c r="C115" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="D115" s="53"/>
+      <c r="D115" s="51"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="51" t="s">
+      <c r="A116" s="49" t="s">
         <v>348</v>
       </c>
-      <c r="B116" s="52" t="s">
+      <c r="B116" s="50" t="s">
         <v>349</v>
       </c>
       <c r="C116" s="9" t="s">
         <v>350</v>
       </c>
-      <c r="D116" s="53" t="s">
+      <c r="D116" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="51"/>
-      <c r="B117" s="52"/>
+      <c r="A117" s="49"/>
+      <c r="B117" s="50"/>
       <c r="C117" s="9"/>
-      <c r="D117" s="53"/>
+      <c r="D117" s="51"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="51"/>
-      <c r="B118" s="52"/>
+      <c r="A118" s="49"/>
+      <c r="B118" s="50"/>
       <c r="C118" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="D118" s="53"/>
+      <c r="D118" s="51"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
@@ -5727,87 +5568,87 @@
       <c r="A139" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="B139" s="52" t="s">
+      <c r="B139" s="50" t="s">
         <v>194</v>
       </c>
       <c r="C139" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="D139" s="53" t="s">
+      <c r="D139" s="51" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="12"/>
-      <c r="B140" s="52"/>
+      <c r="B140" s="50"/>
       <c r="C140" s="9"/>
-      <c r="D140" s="53"/>
+      <c r="D140" s="51"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="B141" s="52"/>
+      <c r="B141" s="50"/>
       <c r="C141" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="D141" s="53"/>
+      <c r="D141" s="51"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="51" t="s">
+      <c r="A142" s="49" t="s">
         <v>397</v>
       </c>
-      <c r="B142" s="52" t="s">
+      <c r="B142" s="50" t="s">
         <v>194</v>
       </c>
       <c r="C142" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="D142" s="53" t="s">
+      <c r="D142" s="51" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="51"/>
-      <c r="B143" s="52"/>
+      <c r="A143" s="49"/>
+      <c r="B143" s="50"/>
       <c r="C143" s="9"/>
-      <c r="D143" s="53"/>
+      <c r="D143" s="51"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="51"/>
-      <c r="B144" s="52"/>
+      <c r="A144" s="49"/>
+      <c r="B144" s="50"/>
       <c r="C144" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="D144" s="53"/>
+      <c r="D144" s="51"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="51" t="s">
+      <c r="A145" s="49" t="s">
         <v>400</v>
       </c>
-      <c r="B145" s="52" t="s">
+      <c r="B145" s="50" t="s">
         <v>187</v>
       </c>
       <c r="C145" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="D145" s="53" t="s">
+      <c r="D145" s="51" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="51"/>
-      <c r="B146" s="52"/>
+      <c r="A146" s="49"/>
+      <c r="B146" s="50"/>
       <c r="C146" s="9"/>
-      <c r="D146" s="53"/>
+      <c r="D146" s="51"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="51"/>
-      <c r="B147" s="52"/>
+      <c r="A147" s="49"/>
+      <c r="B147" s="50"/>
       <c r="C147" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="D147" s="53"/>
+      <c r="D147" s="51"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
@@ -5838,32 +5679,32 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="51" t="s">
+      <c r="A150" s="49" t="s">
         <v>407</v>
       </c>
-      <c r="B150" s="52" t="s">
+      <c r="B150" s="50" t="s">
         <v>408</v>
       </c>
       <c r="C150" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="D150" s="53" t="s">
+      <c r="D150" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="51"/>
-      <c r="B151" s="52"/>
+      <c r="A151" s="49"/>
+      <c r="B151" s="50"/>
       <c r="C151" s="9"/>
-      <c r="D151" s="53"/>
+      <c r="D151" s="51"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="51"/>
-      <c r="B152" s="52"/>
+      <c r="A152" s="49"/>
+      <c r="B152" s="50"/>
       <c r="C152" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="D152" s="53"/>
+      <c r="D152" s="51"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
@@ -5880,60 +5721,60 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="51" t="s">
+      <c r="A154" s="49" t="s">
         <v>413</v>
       </c>
       <c r="B154" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="C154" s="52" t="s">
+      <c r="C154" s="50" t="s">
         <v>416</v>
       </c>
-      <c r="D154" s="53" t="s">
+      <c r="D154" s="51" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="51"/>
+      <c r="A155" s="49"/>
       <c r="B155" s="9"/>
-      <c r="C155" s="52"/>
-      <c r="D155" s="53"/>
+      <c r="C155" s="50"/>
+      <c r="D155" s="51"/>
     </row>
     <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A156" s="51"/>
+      <c r="A156" s="49"/>
       <c r="B156" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="C156" s="52"/>
-      <c r="D156" s="53"/>
+      <c r="C156" s="50"/>
+      <c r="D156" s="51"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="51" t="s">
+      <c r="A157" s="49" t="s">
         <v>417</v>
       </c>
       <c r="B157" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="C157" s="52" t="s">
+      <c r="C157" s="50" t="s">
         <v>420</v>
       </c>
-      <c r="D157" s="53" t="s">
+      <c r="D157" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="51"/>
+      <c r="A158" s="49"/>
       <c r="B158" s="9"/>
-      <c r="C158" s="52"/>
-      <c r="D158" s="53"/>
+      <c r="C158" s="50"/>
+      <c r="D158" s="51"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="51"/>
+      <c r="A159" s="49"/>
       <c r="B159" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="C159" s="52"/>
-      <c r="D159" s="53"/>
+      <c r="C159" s="50"/>
+      <c r="D159" s="51"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
@@ -5964,7 +5805,7 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="51" t="s">
+      <c r="A162" s="49" t="s">
         <v>425</v>
       </c>
       <c r="B162" s="9" t="s">
@@ -5973,53 +5814,53 @@
       <c r="C162" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="D162" s="53" t="s">
+      <c r="D162" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="51"/>
+      <c r="A163" s="49"/>
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
-      <c r="D163" s="53"/>
+      <c r="D163" s="51"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="51"/>
+      <c r="A164" s="49"/>
       <c r="B164" s="9" t="s">
         <v>427</v>
       </c>
       <c r="C164" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="D164" s="53"/>
+      <c r="D164" s="51"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="51"/>
+      <c r="A165" s="49"/>
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
-      <c r="D165" s="53"/>
+      <c r="D165" s="51"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="51"/>
+      <c r="A166" s="49"/>
       <c r="B166" s="9" t="s">
         <v>428</v>
       </c>
       <c r="C166" s="9"/>
-      <c r="D166" s="53"/>
+      <c r="D166" s="51"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="51"/>
+      <c r="A167" s="49"/>
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
-      <c r="D167" s="53"/>
+      <c r="D167" s="51"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="51"/>
+      <c r="A168" s="49"/>
       <c r="B168" s="9" t="s">
         <v>429</v>
       </c>
       <c r="C168" s="9"/>
-      <c r="D168" s="53"/>
+      <c r="D168" s="51"/>
     </row>
     <row r="169" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
@@ -6050,46 +5891,46 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="51" t="s">
+      <c r="A171" s="49" t="s">
         <v>436</v>
       </c>
       <c r="B171" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="C171" s="52" t="s">
+      <c r="C171" s="50" t="s">
         <v>438</v>
       </c>
-      <c r="D171" s="53" t="s">
+      <c r="D171" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="51"/>
+      <c r="A172" s="49"/>
       <c r="B172" s="9"/>
-      <c r="C172" s="52"/>
-      <c r="D172" s="53"/>
+      <c r="C172" s="50"/>
+      <c r="D172" s="51"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="51"/>
+      <c r="A173" s="49"/>
       <c r="B173" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="C173" s="52"/>
-      <c r="D173" s="53"/>
+      <c r="C173" s="50"/>
+      <c r="D173" s="51"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="51"/>
+      <c r="A174" s="49"/>
       <c r="B174" s="9"/>
-      <c r="C174" s="52"/>
-      <c r="D174" s="53"/>
+      <c r="C174" s="50"/>
+      <c r="D174" s="51"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="51"/>
+      <c r="A175" s="49"/>
       <c r="B175" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="C175" s="52"/>
-      <c r="D175" s="53"/>
+      <c r="C175" s="50"/>
+      <c r="D175" s="51"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="12" t="s">
@@ -6120,46 +5961,46 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="51" t="s">
+      <c r="A178" s="49" t="s">
         <v>443</v>
       </c>
-      <c r="B178" s="52" t="s">
+      <c r="B178" s="50" t="s">
         <v>444</v>
       </c>
       <c r="C178" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D178" s="53" t="s">
+      <c r="D178" s="51" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="51"/>
-      <c r="B179" s="52"/>
+      <c r="A179" s="49"/>
+      <c r="B179" s="50"/>
       <c r="C179" s="9"/>
-      <c r="D179" s="53"/>
+      <c r="D179" s="51"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="51"/>
-      <c r="B180" s="52"/>
+      <c r="A180" s="49"/>
+      <c r="B180" s="50"/>
       <c r="C180" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="D180" s="53"/>
+      <c r="D180" s="51"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="51"/>
-      <c r="B181" s="52"/>
+      <c r="A181" s="49"/>
+      <c r="B181" s="50"/>
       <c r="C181" s="9"/>
-      <c r="D181" s="53"/>
+      <c r="D181" s="51"/>
     </row>
     <row r="182" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A182" s="51"/>
-      <c r="B182" s="52"/>
+      <c r="A182" s="49"/>
+      <c r="B182" s="50"/>
       <c r="C182" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="D182" s="53"/>
+      <c r="D182" s="51"/>
     </row>
     <row r="183" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="14" t="s">
@@ -6298,12 +6139,12 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="38" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>467</v>
       </c>
     </row>
@@ -6313,7 +6154,7 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="42" t="s">
         <v>470</v>
       </c>
     </row>
@@ -6328,7 +6169,7 @@
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="47" t="s">
         <v>473</v>
       </c>
     </row>

</xml_diff>